<commit_message>
erstes Beispiel für die Startseite des Programms
</commit_message>
<xml_diff>
--- a/Assets/Dokumentation/WI_Projekt.xlsx
+++ b/Assets/Dokumentation/WI_Projekt.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26207"/>
-  <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MajkenPlugge/Documents/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
+  <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14480" activeTab="1"/>
   </bookViews>
@@ -291,11 +286,11 @@
     </xf>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0" customBuiltin="1"/>
+    <cellStyle name="Titel" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="6">
     <dxf>
@@ -568,7 +563,7 @@
                     </a:solidFill>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="de-DE"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -662,8 +657,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2143969472"/>
-        <c:axId val="-2144064176"/>
+        <c:axId val="2107701576"/>
+        <c:axId val="2107699192"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -768,11 +763,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2121655856"/>
-        <c:axId val="2121652112"/>
+        <c:axId val="2109250504"/>
+        <c:axId val="2107697512"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="2121655856"/>
+        <c:axId val="2109250504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -809,10 +804,10 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2121652112"/>
+        <c:crossAx val="2107697512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -823,7 +818,7 @@
         <c:minorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2121652112"/>
+        <c:axId val="2107697512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -833,12 +828,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2121655856"/>
+        <c:crossAx val="2109250504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2144064176"/>
+        <c:axId val="2107699192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -848,12 +843,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2143969472"/>
+        <c:crossAx val="2107701576"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="-2143969472"/>
+        <c:axId val="2107701576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -863,7 +858,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2144064176"/>
+        <c:crossAx val="2107699192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1352,7 +1347,7 @@
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="3.6640625" customWidth="1"/>
     <col min="2" max="2" width="15.5" customWidth="1"/>
@@ -1366,7 +1361,7 @@
     <col min="14" max="14" width="9.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="24.75" customHeight="1">
       <c r="A1" s="9"/>
       <c r="B1" s="15" t="s">
         <v>8</v>
@@ -1384,7 +1379,7 @@
       <c r="M1" s="9"/>
       <c r="N1" s="9"/>
     </row>
-    <row r="2" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:14" ht="28.5" customHeight="1">
       <c r="A2" s="9"/>
       <c r="B2" s="13" t="s">
         <v>2</v>
@@ -1402,59 +1397,59 @@
       <c r="M2" s="9"/>
       <c r="N2" s="9"/>
     </row>
-    <row r="7" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:14" ht="19.5" customHeight="1">
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:14" ht="19.5" customHeight="1">
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:14" ht="19.5" customHeight="1">
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:14" ht="19.5" customHeight="1">
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:14" ht="19.5" customHeight="1">
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:14" ht="19.5" customHeight="1">
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:14" ht="19.5" customHeight="1">
       <c r="F13" s="1"/>
       <c r="I13" s="2"/>
       <c r="K13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="3"/>
     </row>
-    <row r="14" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:14" ht="19.5" customHeight="1">
       <c r="F14" s="1"/>
       <c r="I14" s="2"/>
       <c r="K14" s="2"/>
       <c r="M14" s="2"/>
       <c r="N14" s="3"/>
     </row>
-    <row r="15" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:14" ht="19.5" customHeight="1">
       <c r="F15" s="1"/>
       <c r="I15" s="2"/>
       <c r="K15" s="2"/>
       <c r="M15" s="2"/>
       <c r="N15" s="3"/>
     </row>
-    <row r="16" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:14" ht="19.5" customHeight="1">
       <c r="F16" s="1"/>
       <c r="I16" s="2"/>
       <c r="K16" s="2"/>
       <c r="M16" s="2"/>
       <c r="N16" s="3"/>
     </row>
-    <row r="17" spans="2:14" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:14" ht="19.5" customHeight="1" thickBot="1">
       <c r="I17" s="2"/>
       <c r="K17" s="2"/>
       <c r="M17" s="2"/>
       <c r="N17" s="3"/>
     </row>
-    <row r="18" spans="2:14" ht="24" customHeight="1" thickTop="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:14" ht="24" customHeight="1" thickTop="1">
       <c r="B18" s="10" t="s">
         <v>7</v>
       </c>
@@ -1465,7 +1460,7 @@
       <c r="M18" s="2"/>
       <c r="N18" s="3"/>
     </row>
-    <row r="19" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:14" ht="24" customHeight="1">
       <c r="B19" s="6" t="s">
         <v>3</v>
       </c>
@@ -1484,7 +1479,7 @@
       <c r="M19" s="2"/>
       <c r="N19" s="3"/>
     </row>
-    <row r="20" spans="2:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:14" ht="19.5" customHeight="1">
       <c r="B20" s="14">
         <v>42254</v>
       </c>
@@ -1503,7 +1498,7 @@
       <c r="M20" s="2"/>
       <c r="N20" s="3"/>
     </row>
-    <row r="21" spans="2:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:14" ht="19.5" customHeight="1">
       <c r="B21" s="14">
         <v>42275</v>
       </c>
@@ -1523,7 +1518,7 @@
       <c r="M21" s="2"/>
       <c r="N21" s="3"/>
     </row>
-    <row r="22" spans="2:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:14" ht="19.5" customHeight="1">
       <c r="B22" s="14">
         <v>42296</v>
       </c>
@@ -1542,7 +1537,7 @@
       <c r="M22" s="2"/>
       <c r="N22" s="3"/>
     </row>
-    <row r="23" spans="2:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:14" ht="19.5" customHeight="1">
       <c r="B23" s="14">
         <v>42317</v>
       </c>
@@ -1561,7 +1556,7 @@
       <c r="M23" s="2"/>
       <c r="N23" s="3"/>
     </row>
-    <row r="24" spans="2:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="2:14" ht="19.5" customHeight="1">
       <c r="B24" s="14">
         <v>42317</v>
       </c>
@@ -1580,28 +1575,33 @@
       <c r="M24" s="2"/>
       <c r="N24" s="3"/>
     </row>
-    <row r="25" spans="2:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="2:14" ht="19.5" customHeight="1">
       <c r="I25" s="2"/>
       <c r="K25" s="2"/>
       <c r="M25" s="2"/>
       <c r="N25" s="3"/>
     </row>
-    <row r="26" spans="2:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="2:14" ht="19.5" customHeight="1">
       <c r="I26" s="2"/>
       <c r="K26" s="2"/>
       <c r="M26" s="2"/>
       <c r="N26" s="3"/>
     </row>
-    <row r="29" spans="2:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="2:14" ht="19.5" customHeight="1">
       <c r="H29" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" fitToHeight="0" orientation="landscape" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" fitToHeight="0" orientation="landscape"/>
+  <drawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1610,10 +1610,10 @@
   <dimension ref="B2:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="16"/>
     <col min="2" max="2" width="16.6640625" style="16" customWidth="1"/>
@@ -1624,7 +1624,7 @@
     <col min="7" max="16384" width="10.83203125" style="16"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:6">
       <c r="B2" s="16" t="s">
         <v>12</v>
       </c>
@@ -1641,7 +1641,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="3" spans="2:6">
       <c r="B3" s="16" t="s">
         <v>17</v>
       </c>
@@ -1652,7 +1652,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:6">
       <c r="B4" s="16" t="s">
         <v>19</v>
       </c>
@@ -1663,7 +1663,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:6">
       <c r="B5" s="16" t="s">
         <v>21</v>
       </c>
@@ -1674,7 +1674,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:6">
       <c r="B6" s="16" t="s">
         <v>23</v>
       </c>
@@ -1685,7 +1685,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="7" spans="2:6">
       <c r="B7" s="16" t="s">
         <v>25</v>
       </c>
@@ -1698,6 +1698,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1709,7 +1714,7 @@
       <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="2" width="10.83203125" style="16"/>
     <col min="3" max="3" width="14.83203125" style="16" customWidth="1"/>
@@ -1719,7 +1724,7 @@
     <col min="7" max="16384" width="10.83203125" style="16"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:6">
       <c r="B2" s="16" t="s">
         <v>12</v>
       </c>
@@ -1738,6 +1743,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1749,7 +1759,7 @@
       <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="2" width="10.83203125" style="16"/>
     <col min="3" max="3" width="14.83203125" style="16" customWidth="1"/>
@@ -1759,7 +1769,7 @@
     <col min="7" max="16384" width="10.83203125" style="16"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.15">
+    <row r="2" spans="2:6">
       <c r="B2" s="16" t="s">
         <v>12</v>
       </c>
@@ -1778,6 +1788,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
WI-Projektplan E/R Modellerieung Update Datenbank Update
</commit_message>
<xml_diff>
--- a/Assets/Dokumentation/WI_Projekt.xlsx
+++ b/Assets/Dokumentation/WI_Projekt.xlsx
@@ -1,23 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
-  <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26311"/>
+  <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MajkenPlugge/Documents/DHBW/5.Semester/WI_Projekt/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14000"/>
   </bookViews>
   <sheets>
-    <sheet name="GANT" sheetId="1" r:id="rId1"/>
+    <sheet name="Zeitachse" sheetId="1" r:id="rId1"/>
     <sheet name="1. Prototyp" sheetId="11" r:id="rId2"/>
     <sheet name="2. Beta-Version" sheetId="2" r:id="rId3"/>
     <sheet name="3. Endtunier" sheetId="12" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">GANT!$A$1:$N$17</definedName>
-    <definedName name="Projektende">GANT!$L$21</definedName>
-    <definedName name="Projektstart">GANT!$L$19</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Zeitachse!$A$1:$N$17</definedName>
+    <definedName name="Projektende">Zeitachse!$L$21</definedName>
+    <definedName name="Projektstart">Zeitachse!$L$19</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -89,6 +94,9 @@
     <t>Cara Damm</t>
   </si>
   <si>
+    <t>Mockups erstellen</t>
+  </si>
+  <si>
     <t xml:space="preserve">Alexander Kern </t>
   </si>
   <si>
@@ -109,19 +117,16 @@
   <si>
     <t>Aktivitätendiagramm</t>
   </si>
-  <si>
-    <t>Mockups erstellen + UI Entwerfen</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1" tint="0.499984740745262"/>
-      <name val="Arial Rounded MT Bold"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -129,7 +134,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial Rounded MT Bold"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -137,7 +142,7 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="Arial Rounded MT Bold"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -145,14 +150,14 @@
       <b/>
       <sz val="20"/>
       <color theme="0"/>
-      <name val="Arial Rounded MT Bold"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="5"/>
-      <name val="Arial Rounded MT Bold"/>
+      <name val="Arial Black"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
@@ -160,23 +165,7 @@
       <b/>
       <sz val="11"/>
       <color theme="5"/>
-      <name val="Arial Rounded MT Bold"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color theme="10"/>
-      <name val="Arial Rounded MT Bold"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color theme="11"/>
-      <name val="Arial Rounded MT Bold"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -241,7 +230,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="59">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -249,168 +238,6 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0">
@@ -463,66 +290,12 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="59">
-    <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Titel" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
+  <cellStyles count="5">
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="6">
     <dxf>
@@ -629,7 +402,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>GANT!$D$19</c:f>
+              <c:f>Zeitachse!$D$19</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -795,7 +568,7 @@
                     </a:solidFill>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="de-DE"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -834,7 +607,7 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>GANT!$C$20:$C$25</c:f>
+              <c:f>Zeitachse!$C$20:$C$25</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -857,7 +630,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>GANT!$D$20:$D$25</c:f>
+              <c:f>Zeitachse!$D$20:$D$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -889,8 +662,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2108525960"/>
-        <c:axId val="2108523016"/>
+        <c:axId val="-2068068176"/>
+        <c:axId val="-2068070672"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -900,7 +673,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>GANT!$B$19</c:f>
+              <c:f>Zeitachse!$B$19</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -937,7 +710,7 @@
           </c:errBars>
           <c:cat>
             <c:numRef>
-              <c:f>GANT!$B$20:$B$25</c:f>
+              <c:f>Zeitachse!$B$20:$B$25</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
                 <c:ptCount val="6"/>
@@ -961,7 +734,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>GANT!$E$20:$E$25</c:f>
+              <c:f>Zeitachse!$E$20:$E$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -995,11 +768,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2109166712"/>
-        <c:axId val="2108519912"/>
+        <c:axId val="-2068076672"/>
+        <c:axId val="-2068073248"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="2109166712"/>
+        <c:axId val="-2068076672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1036,10 +809,10 @@
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2108519912"/>
+        <c:crossAx val="-2068073248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -1050,7 +823,7 @@
         <c:minorTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2108519912"/>
+        <c:axId val="-2068073248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1060,12 +833,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2109166712"/>
+        <c:crossAx val="-2068076672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2108523016"/>
+        <c:axId val="-2068070672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1075,12 +848,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2108525960"/>
+        <c:crossAx val="-2068068176"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="2108525960"/>
+        <c:axId val="-2068068176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1090,7 +863,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2108523016"/>
+        <c:crossAx val="-2068070672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1343,79 +1116,91 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Himmel">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Amphitrite">
+    <a:clrScheme name="Project Timeline_1">
       <a:dk1>
-        <a:srgbClr val="302C24"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="AC6416"/>
+        <a:srgbClr val="2A2C3B"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E8E4DB"/>
+        <a:srgbClr val="FBFCF4"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="C6B178"/>
+        <a:srgbClr val="F65242"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="9C5B14"/>
+        <a:srgbClr val="70B5CF"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="71B2BC"/>
+        <a:srgbClr val="A78400"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="78AA5D"/>
+        <a:srgbClr val="60B6AC"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="867099"/>
+        <a:srgbClr val="ED9535"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="4C6F75"/>
+        <a:srgbClr val="AD7A99"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="F27B0E"/>
+        <a:srgbClr val="70B5CF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="989268"/>
+        <a:srgbClr val="AD7A99"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Himmel">
+    <a:fontScheme name="Project Timeline">
       <a:majorFont>
-        <a:latin typeface="Arial Rounded MT Bold"/>
+        <a:latin typeface="Arial Black"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Arial Rounded MT Bold"/>
+        <a:latin typeface="Arial"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Himmel">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:alpha val="50000"/>
-          </a:schemeClr>
         </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
@@ -1432,11 +1217,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="14400000" scaled="1"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -1445,13 +1230,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="31750" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="63500" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1460,11 +1245,17 @@
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="88900" dist="63500" dir="3000000" algn="br" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1473,13 +1264,23 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:innerShdw blurRad="50800" dist="25400" dir="6600000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="50000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
-            </a:innerShdw>
-            <a:reflection blurRad="12700" stA="26000" endPos="28000" dist="38100" dir="5400000" sy="-100000" rotWithShape="0"/>
+            </a:outerShdw>
           </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
@@ -1490,21 +1291,26 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
-                <a:satMod val="140000"/>
-                <a:lumMod val="105000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:shade val="20000"/>
-                <a:satMod val="250000"/>
-                <a:lumMod val="110000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -1522,7 +1328,9 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
@@ -1540,11 +1348,11 @@
   </sheetPr>
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A14" zoomScale="101" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="101" workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="3.6640625" customWidth="1"/>
     <col min="2" max="2" width="15.5" customWidth="1"/>
@@ -1558,7 +1366,7 @@
     <col min="14" max="14" width="9.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="24.75" customHeight="1">
+    <row r="1" spans="1:14" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9"/>
       <c r="B1" s="15" t="s">
         <v>8</v>
@@ -1576,7 +1384,7 @@
       <c r="M1" s="9"/>
       <c r="N1" s="9"/>
     </row>
-    <row r="2" spans="1:14" ht="28.5" customHeight="1">
+    <row r="2" spans="1:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="9"/>
       <c r="B2" s="13" t="s">
         <v>2</v>
@@ -1594,59 +1402,59 @@
       <c r="M2" s="9"/>
       <c r="N2" s="9"/>
     </row>
-    <row r="7" spans="1:14" ht="19.5" customHeight="1">
+    <row r="7" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:14" ht="19.5" customHeight="1">
+    <row r="8" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:14" ht="19.5" customHeight="1">
+    <row r="9" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:14" ht="19.5" customHeight="1">
+    <row r="10" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:14" ht="19.5" customHeight="1">
+    <row r="11" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:14" ht="19.5" customHeight="1">
+    <row r="12" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:14" ht="19.5" customHeight="1">
+    <row r="13" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F13" s="1"/>
       <c r="I13" s="2"/>
       <c r="K13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="3"/>
     </row>
-    <row r="14" spans="1:14" ht="19.5" customHeight="1">
+    <row r="14" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F14" s="1"/>
       <c r="I14" s="2"/>
       <c r="K14" s="2"/>
       <c r="M14" s="2"/>
       <c r="N14" s="3"/>
     </row>
-    <row r="15" spans="1:14" ht="19.5" customHeight="1">
+    <row r="15" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F15" s="1"/>
       <c r="I15" s="2"/>
       <c r="K15" s="2"/>
       <c r="M15" s="2"/>
       <c r="N15" s="3"/>
     </row>
-    <row r="16" spans="1:14" ht="19.5" customHeight="1">
+    <row r="16" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F16" s="1"/>
       <c r="I16" s="2"/>
       <c r="K16" s="2"/>
       <c r="M16" s="2"/>
       <c r="N16" s="3"/>
     </row>
-    <row r="17" spans="2:14" ht="19.5" customHeight="1" thickBot="1">
+    <row r="17" spans="2:14" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="I17" s="2"/>
       <c r="K17" s="2"/>
       <c r="M17" s="2"/>
       <c r="N17" s="3"/>
     </row>
-    <row r="18" spans="2:14" ht="24" customHeight="1" thickTop="1">
+    <row r="18" spans="2:14" ht="24" customHeight="1" thickTop="1" x14ac:dyDescent="0.15">
       <c r="B18" s="10" t="s">
         <v>7</v>
       </c>
@@ -1657,7 +1465,7 @@
       <c r="M18" s="2"/>
       <c r="N18" s="3"/>
     </row>
-    <row r="19" spans="2:14" ht="24" customHeight="1">
+    <row r="19" spans="2:14" ht="24" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="6" t="s">
         <v>3</v>
       </c>
@@ -1676,7 +1484,7 @@
       <c r="M19" s="2"/>
       <c r="N19" s="3"/>
     </row>
-    <row r="20" spans="2:14" ht="19.5" customHeight="1">
+    <row r="20" spans="2:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="14">
         <v>42254</v>
       </c>
@@ -1695,7 +1503,7 @@
       <c r="M20" s="2"/>
       <c r="N20" s="3"/>
     </row>
-    <row r="21" spans="2:14" ht="19.5" customHeight="1">
+    <row r="21" spans="2:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="14">
         <v>42275</v>
       </c>
@@ -1715,7 +1523,7 @@
       <c r="M21" s="2"/>
       <c r="N21" s="3"/>
     </row>
-    <row r="22" spans="2:14" ht="19.5" customHeight="1">
+    <row r="22" spans="2:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="14">
         <v>42296</v>
       </c>
@@ -1734,7 +1542,7 @@
       <c r="M22" s="2"/>
       <c r="N22" s="3"/>
     </row>
-    <row r="23" spans="2:14" ht="19.5" customHeight="1">
+    <row r="23" spans="2:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" s="14">
         <v>42317</v>
       </c>
@@ -1753,7 +1561,7 @@
       <c r="M23" s="2"/>
       <c r="N23" s="3"/>
     </row>
-    <row r="24" spans="2:14" ht="19.5" customHeight="1">
+    <row r="24" spans="2:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="14">
         <v>42317</v>
       </c>
@@ -1772,33 +1580,28 @@
       <c r="M24" s="2"/>
       <c r="N24" s="3"/>
     </row>
-    <row r="25" spans="2:14" ht="19.5" customHeight="1">
+    <row r="25" spans="2:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="I25" s="2"/>
       <c r="K25" s="2"/>
       <c r="M25" s="2"/>
       <c r="N25" s="3"/>
     </row>
-    <row r="26" spans="2:14" ht="19.5" customHeight="1">
+    <row r="26" spans="2:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="I26" s="2"/>
       <c r="K26" s="2"/>
       <c r="M26" s="2"/>
       <c r="N26" s="3"/>
     </row>
-    <row r="29" spans="2:14" ht="19.5" customHeight="1">
+    <row r="29" spans="2:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="H29" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" fitToHeight="0" orientation="landscape"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1806,13 +1609,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:F17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="16" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="16"/>
     <col min="2" max="2" width="16.6640625" style="16" customWidth="1"/>
     <col min="3" max="3" width="23.33203125" style="16" customWidth="1"/>
     <col min="4" max="4" width="23.5" style="16" customWidth="1"/>
@@ -1821,7 +1624,7 @@
     <col min="7" max="16384" width="10.83203125" style="16"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B2" s="16" t="s">
         <v>12</v>
       </c>
@@ -1829,7 +1632,7 @@
         <v>13</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E2" s="16" t="s">
         <v>15</v>
@@ -1838,7 +1641,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="2:6">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B3" s="16" t="s">
         <v>17</v>
       </c>
@@ -1849,48 +1652,45 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:6">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B4" s="16" t="s">
         <v>19</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="D4" s="16">
         <v>3</v>
       </c>
-      <c r="E4" s="16">
-        <v>14</v>
-      </c>
     </row>
-    <row r="5" spans="2:6">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B5" s="16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D5" s="16">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:6">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B6" s="16" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D6" s="16">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:6">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B7" s="16" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D7" s="16">
         <v>3</v>
@@ -1898,12 +1698,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1915,7 +1709,7 @@
       <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="2" width="10.83203125" style="16"/>
     <col min="3" max="3" width="14.83203125" style="16" customWidth="1"/>
@@ -1925,7 +1719,7 @@
     <col min="7" max="16384" width="10.83203125" style="16"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B2" s="16" t="s">
         <v>12</v>
       </c>
@@ -1944,11 +1738,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1960,7 +1749,7 @@
       <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="2" width="10.83203125" style="16"/>
     <col min="3" max="3" width="14.83203125" style="16" customWidth="1"/>
@@ -1970,7 +1759,7 @@
     <col min="7" max="16384" width="10.83203125" style="16"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B2" s="16" t="s">
         <v>12</v>
       </c>
@@ -1989,15 +1778,147 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType encoding="utf-8"?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>AssetEditForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <MarketSpecific xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">false</MarketSpecific>
+    <ApprovalStatus xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">InProgress</ApprovalStatus>
+    <LocComments xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
+    <DirectSourceMarket xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">english</DirectSourceMarket>
+    <ThumbnailAssetId xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
+    <PrimaryImageGen xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">false</PrimaryImageGen>
+    <LegacyData xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
+    <TPFriendlyName xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
+    <NumericId xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
+    <LocRecommendedHandoff xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
+    <BlockPublish xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">false</BlockPublish>
+    <BusinessGroup xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
+    <OpenTemplate xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">true</OpenTemplate>
+    <SourceTitle xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
+    <APEditor xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </APEditor>
+    <UALocComments xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
+    <FeatureTagsTaxHTField0 xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </FeatureTagsTaxHTField0>
+    <IntlLangReviewDate xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
+    <PublishStatusLookup xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">
+      <Value>560172</Value>
+    </PublishStatusLookup>
+    <ParentAssetId xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
+    <MachineTranslated xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">false</MachineTranslated>
+    <Providers xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
+    <OriginalSourceMarket xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">english</OriginalSourceMarket>
+    <APDescription xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
+    <ContentItem xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
+    <ClipArtFilename xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
+    <TPInstallLocation xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
+    <TimesCloned xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
+    <PublishTargets xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">OfficeOnlineVNext</PublishTargets>
+    <AcquiredFrom xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">Internal MS</AcquiredFrom>
+    <AssetStart xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">2012-06-28T22:28:00+00:00</AssetStart>
+    <FriendlyTitle xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
+    <Provider xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
+    <LastHandOff xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
+    <Manager xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
+    <UALocRecommendation xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">Localize</UALocRecommendation>
+    <ArtSampleDocs xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
+    <UACurrentWords xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
+    <TPClientViewer xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
+    <TemplateStatus xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">Complete</TemplateStatus>
+    <ShowIn xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">Show everywhere</ShowIn>
+    <CSXHash xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
+    <Downloads xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">0</Downloads>
+    <VoteCount xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
+    <OOCacheId xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
+    <IsDeleted xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">false</IsDeleted>
+    <InternalTagsTaxHTField0 xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </InternalTagsTaxHTField0>
+    <UANotes xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
+    <AssetExpire xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">2029-01-01T08:00:00+00:00</AssetExpire>
+    <CSXSubmissionMarket xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
+    <DSATActionTaken xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
+    <SubmitterId xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
+    <EditorialTags xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
+    <TPExecutable xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
+    <CSXSubmissionDate xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
+    <CSXUpdate xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">false</CSXUpdate>
+    <AssetType xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">TP</AssetType>
+    <ApprovalLog xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
+    <BugNumber xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
+    <OriginAsset xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
+    <TPComponent xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
+    <Milestone xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
+    <RecommendationsModifier xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
+    <AssetId xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">TP102929982</AssetId>
+    <PolicheckWords xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
+    <TPLaunchHelpLink xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
+    <IntlLocPriority xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
+    <TPApplication xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
+    <CrawlForDependencies xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">false</CrawlForDependencies>
+    <IntlLangReviewer xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
+    <HandoffToMSDN xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
+    <PlannedPubDate xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
+    <LocLastLocAttemptVersionLookup xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">845888</LocLastLocAttemptVersionLookup>
+    <TrustLevel xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">1 Microsoft Managed Content</TrustLevel>
+    <CampaignTagsTaxHTField0 xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </CampaignTagsTaxHTField0>
+    <TPNamespace xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
+    <TaxCatchAll xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f"/>
+    <IsSearchable xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">false</IsSearchable>
+    <TemplateTemplateType xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">Excel Spreadsheet Template</TemplateTemplateType>
+    <Markets xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f"/>
+    <IntlLangReview xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">false</IntlLangReview>
+    <UAProjectedTotalWords xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
+    <OutputCachingOn xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">false</OutputCachingOn>
+    <LocMarketGroupTiers2 xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
+    <AverageRating xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
+    <APAuthor xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">
+      <UserInfo>
+        <DisplayName>REDMOND\v-aptall</DisplayName>
+        <AccountId>2566</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </APAuthor>
+    <TPCommandLine xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
+    <LocManualTestRequired xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">false</LocManualTestRequired>
+    <TPAppVersion xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
+    <EditorialStatus xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
+    <LastModifiedDateTime xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
+    <TPLaunchHelpLinkType xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">Template</TPLaunchHelpLinkType>
+    <OriginalRelease xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">15</OriginalRelease>
+    <ScenarioTagsTaxHTField0 xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ScenarioTagsTaxHTField0>
+    <LocalizationTagsTaxHTField0 xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </LocalizationTagsTaxHTField0>
+    <Component xmlns="c7af2036-029c-470e-8042-297c68a41472" xsi:nil="true"/>
+    <Description0 xmlns="c7af2036-029c-470e-8042-297c68a41472" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="TemplateFile" ma:contentTypeID="0x01010037696D9D1D95EC45A9440548E782419D04008C4669C20C93454ABB50E332FADBDDBE" ma:contentTypeVersion="55" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="0862fa1d3c98dca9116b8c2bbf050b2c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xmlns:ns3="c7af2036-029c-470e-8042-297c68a41472" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="efcf89ea05a71204977c7c6a0a118372" ns2:_="" ns3:_="">
     <xsd:import namespace="f105ad54-119a-4495-aa55-0e28b6b4ad2f"/>
@@ -3056,144 +2977,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType encoding="utf-8"?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>AssetEditForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E799163A-BF88-4F66-AA5F-07DF46097E18}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <MarketSpecific xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">false</MarketSpecific>
-    <ApprovalStatus xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">InProgress</ApprovalStatus>
-    <LocComments xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
-    <DirectSourceMarket xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">english</DirectSourceMarket>
-    <ThumbnailAssetId xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
-    <PrimaryImageGen xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">false</PrimaryImageGen>
-    <LegacyData xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
-    <TPFriendlyName xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
-    <NumericId xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
-    <LocRecommendedHandoff xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
-    <BlockPublish xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">false</BlockPublish>
-    <BusinessGroup xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
-    <OpenTemplate xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">true</OpenTemplate>
-    <SourceTitle xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
-    <APEditor xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </APEditor>
-    <UALocComments xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
-    <FeatureTagsTaxHTField0 xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </FeatureTagsTaxHTField0>
-    <IntlLangReviewDate xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
-    <PublishStatusLookup xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">
-      <Value>560172</Value>
-    </PublishStatusLookup>
-    <ParentAssetId xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
-    <MachineTranslated xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">false</MachineTranslated>
-    <Providers xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
-    <OriginalSourceMarket xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">english</OriginalSourceMarket>
-    <APDescription xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
-    <ContentItem xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
-    <ClipArtFilename xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
-    <TPInstallLocation xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
-    <TimesCloned xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
-    <PublishTargets xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">OfficeOnlineVNext</PublishTargets>
-    <AcquiredFrom xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">Internal MS</AcquiredFrom>
-    <AssetStart xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">2012-06-28T22:28:00+00:00</AssetStart>
-    <FriendlyTitle xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
-    <Provider xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
-    <LastHandOff xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
-    <Manager xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
-    <UALocRecommendation xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">Localize</UALocRecommendation>
-    <ArtSampleDocs xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
-    <UACurrentWords xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
-    <TPClientViewer xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
-    <TemplateStatus xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">Complete</TemplateStatus>
-    <ShowIn xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">Show everywhere</ShowIn>
-    <CSXHash xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
-    <Downloads xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">0</Downloads>
-    <VoteCount xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
-    <OOCacheId xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
-    <IsDeleted xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">false</IsDeleted>
-    <InternalTagsTaxHTField0 xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </InternalTagsTaxHTField0>
-    <UANotes xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
-    <AssetExpire xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">2029-01-01T08:00:00+00:00</AssetExpire>
-    <CSXSubmissionMarket xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
-    <DSATActionTaken xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
-    <SubmitterId xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
-    <EditorialTags xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
-    <TPExecutable xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
-    <CSXSubmissionDate xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
-    <CSXUpdate xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">false</CSXUpdate>
-    <AssetType xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">TP</AssetType>
-    <ApprovalLog xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
-    <BugNumber xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
-    <OriginAsset xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
-    <TPComponent xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
-    <Milestone xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
-    <RecommendationsModifier xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
-    <AssetId xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">TP102929982</AssetId>
-    <PolicheckWords xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
-    <TPLaunchHelpLink xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
-    <IntlLocPriority xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
-    <TPApplication xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
-    <CrawlForDependencies xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">false</CrawlForDependencies>
-    <IntlLangReviewer xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
-    <HandoffToMSDN xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
-    <PlannedPubDate xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
-    <LocLastLocAttemptVersionLookup xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">845888</LocLastLocAttemptVersionLookup>
-    <TrustLevel xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">1 Microsoft Managed Content</TrustLevel>
-    <CampaignTagsTaxHTField0 xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </CampaignTagsTaxHTField0>
-    <TPNamespace xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
-    <TaxCatchAll xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f"/>
-    <IsSearchable xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">false</IsSearchable>
-    <TemplateTemplateType xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">Excel Spreadsheet Template</TemplateTemplateType>
-    <Markets xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f"/>
-    <IntlLangReview xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">false</IntlLangReview>
-    <UAProjectedTotalWords xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
-    <OutputCachingOn xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">false</OutputCachingOn>
-    <LocMarketGroupTiers2 xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
-    <AverageRating xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
-    <APAuthor xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">
-      <UserInfo>
-        <DisplayName>REDMOND\v-aptall</DisplayName>
-        <AccountId>2566</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </APAuthor>
-    <TPCommandLine xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
-    <LocManualTestRequired xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">false</LocManualTestRequired>
-    <TPAppVersion xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
-    <EditorialStatus xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
-    <LastModifiedDateTime xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f" xsi:nil="true"/>
-    <TPLaunchHelpLinkType xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">Template</TPLaunchHelpLinkType>
-    <OriginalRelease xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">15</OriginalRelease>
-    <ScenarioTagsTaxHTField0 xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ScenarioTagsTaxHTField0>
-    <LocalizationTagsTaxHTField0 xmlns="f105ad54-119a-4495-aa55-0e28b6b4ad2f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </LocalizationTagsTaxHTField0>
-    <Component xmlns="c7af2036-029c-470e-8042-297c68a41472" xsi:nil="true"/>
-    <Description0 xmlns="c7af2036-029c-470e-8042-297c68a41472" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67FD8875-247A-4694-A47F-4C4391686C6A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="f105ad54-119a-4495-aa55-0e28b6b4ad2f"/>
+    <ds:schemaRef ds:uri="c7af2036-029c-470e-8042-297c68a41472"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C35687F7-2804-472E-B8AF-428C37C40FF9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3210,23 +3013,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E799163A-BF88-4F66-AA5F-07DF46097E18}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67FD8875-247A-4694-A47F-4C4391686C6A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="f105ad54-119a-4495-aa55-0e28b6b4ad2f"/>
-    <ds:schemaRef ds:uri="c7af2036-029c-470e-8042-297c68a41472"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>